<commit_message>
versão 1.0 - Inicial do projeto
</commit_message>
<xml_diff>
--- a/ControleFinanceiro.xlsx
+++ b/ControleFinanceiro.xlsx
@@ -17,13 +17,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,81 +429,48 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Descrição</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Valor</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Data de Vencimento</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Data que foi pago</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Valor pago</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Devendo</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>cartão</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>60</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>16/03</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>50</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>PG</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
         </is>
       </c>
     </row>
     <row r="13">
+      <c r="H13" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
       <c r="I13">
         <f>SUM(F2:B50)</f>
         <v/>

</xml_diff>